<commit_message>
Updated Tests for Comments app
</commit_message>
<xml_diff>
--- a/Tests for Comments application Volodya.xlsx
+++ b/Tests for Comments application Volodya.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\V_Ghost\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\V_Ghost\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" tabRatio="620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9165" tabRatio="620" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="6" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="220">
   <si>
     <t>TC_ New Comments page creating - Functional Categories</t>
   </si>
@@ -832,11 +832,26 @@
     <t>Must change category status without
 blinks</t>
   </si>
+  <si>
+    <t>We don`t know, which fonts must be</t>
+  </si>
+  <si>
+    <t>Test case steps can`t contain 
+word "Verify"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case steps can`t contain 
+word "Verify" </t>
+  </si>
+  <si>
+    <t>Test case step can`t contain 
+word "Verify"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1763,6 +1778,45 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1781,126 +1835,114 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1922,39 +1964,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="2" builtinId="10"/>
+    <cellStyle name="Гіперпосилання" xfId="3" builtinId="8"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
+    <cellStyle name="Контрольна клітинка" xfId="1" builtinId="23"/>
+    <cellStyle name="Примітка" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="70">
     <dxf>
@@ -2678,9 +2693,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Офіс">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2718,7 +2733,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Офіс">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2790,7 +2805,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Офіс">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2942,7 +2957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15:Q15"/>
     </sheetView>
   </sheetViews>
@@ -2952,264 +2967,264 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="88"/>
-      <c r="O1" s="88"/>
-      <c r="P1" s="88"/>
-      <c r="Q1" s="88"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
+      <c r="I1" s="101"/>
+      <c r="J1" s="101"/>
+      <c r="K1" s="101"/>
+      <c r="L1" s="101"/>
+      <c r="M1" s="101"/>
+      <c r="N1" s="101"/>
+      <c r="O1" s="101"/>
+      <c r="P1" s="101"/>
+      <c r="Q1" s="101"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="96" t="s">
         <v>166</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="85"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
+      <c r="Q2" s="98"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="86"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="86"/>
-      <c r="Q3" s="87"/>
+      <c r="A3" s="99"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
+      <c r="P3" s="99"/>
+      <c r="Q3" s="100"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="86"/>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="86"/>
-      <c r="Q4" s="87"/>
+      <c r="A4" s="99"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="99"/>
+      <c r="M4" s="99"/>
+      <c r="N4" s="99"/>
+      <c r="O4" s="99"/>
+      <c r="P4" s="99"/>
+      <c r="Q4" s="100"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="86"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="86"/>
-      <c r="J5" s="86"/>
-      <c r="K5" s="86"/>
-      <c r="L5" s="86"/>
-      <c r="M5" s="86"/>
-      <c r="N5" s="86"/>
-      <c r="O5" s="86"/>
-      <c r="P5" s="86"/>
-      <c r="Q5" s="87"/>
+      <c r="A5" s="99"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="99"/>
+      <c r="J5" s="99"/>
+      <c r="K5" s="99"/>
+      <c r="L5" s="99"/>
+      <c r="M5" s="99"/>
+      <c r="N5" s="99"/>
+      <c r="O5" s="99"/>
+      <c r="P5" s="99"/>
+      <c r="Q5" s="100"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="86" t="s">
+      <c r="A6" s="99" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="86"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="86"/>
-      <c r="L6" s="86"/>
-      <c r="M6" s="86"/>
-      <c r="N6" s="86"/>
-      <c r="O6" s="86"/>
-      <c r="P6" s="86"/>
-      <c r="Q6" s="87"/>
+      <c r="B6" s="99"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="99"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="99"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
+      <c r="M6" s="99"/>
+      <c r="N6" s="99"/>
+      <c r="O6" s="99"/>
+      <c r="P6" s="99"/>
+      <c r="Q6" s="100"/>
     </row>
     <row r="7" spans="1:17" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="90" t="s">
+      <c r="B7" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="90"/>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="90"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="90" t="s">
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="94"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="94"/>
+      <c r="L7" s="94"/>
+      <c r="M7" s="94"/>
+      <c r="N7" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="O7" s="90"/>
-      <c r="P7" s="90"/>
-      <c r="Q7" s="90"/>
+      <c r="O7" s="94"/>
+      <c r="P7" s="94"/>
+      <c r="Q7" s="94"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>301</v>
       </c>
-      <c r="B8" s="89" t="s">
+      <c r="B8" s="91" t="s">
         <v>167</v>
       </c>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="89"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="89"/>
-      <c r="J8" s="89"/>
-      <c r="K8" s="89"/>
-      <c r="L8" s="89"/>
-      <c r="M8" s="89"/>
-      <c r="N8" s="89"/>
-      <c r="O8" s="89"/>
-      <c r="P8" s="89"/>
-      <c r="Q8" s="89"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="91"/>
+      <c r="G8" s="91"/>
+      <c r="H8" s="91"/>
+      <c r="I8" s="91"/>
+      <c r="J8" s="91"/>
+      <c r="K8" s="91"/>
+      <c r="L8" s="91"/>
+      <c r="M8" s="91"/>
+      <c r="N8" s="91"/>
+      <c r="O8" s="91"/>
+      <c r="P8" s="91"/>
+      <c r="Q8" s="91"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>302</v>
       </c>
-      <c r="B9" s="89" t="s">
+      <c r="B9" s="91" t="s">
         <v>168</v>
       </c>
-      <c r="C9" s="89"/>
-      <c r="D9" s="89"/>
-      <c r="E9" s="89"/>
-      <c r="F9" s="89"/>
-      <c r="G9" s="89"/>
-      <c r="H9" s="89"/>
-      <c r="I9" s="89"/>
-      <c r="J9" s="89"/>
-      <c r="K9" s="89"/>
-      <c r="L9" s="89"/>
-      <c r="M9" s="89"/>
-      <c r="N9" s="89"/>
-      <c r="O9" s="89"/>
-      <c r="P9" s="89"/>
-      <c r="Q9" s="89"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="91"/>
+      <c r="G9" s="91"/>
+      <c r="H9" s="91"/>
+      <c r="I9" s="91"/>
+      <c r="J9" s="91"/>
+      <c r="K9" s="91"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="91"/>
+      <c r="N9" s="91"/>
+      <c r="O9" s="91"/>
+      <c r="P9" s="91"/>
+      <c r="Q9" s="91"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>303</v>
       </c>
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="91" t="s">
         <v>169</v>
       </c>
-      <c r="C10" s="89"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="89"/>
-      <c r="I10" s="89"/>
-      <c r="J10" s="89"/>
-      <c r="K10" s="89"/>
-      <c r="L10" s="89"/>
-      <c r="M10" s="89"/>
-      <c r="N10" s="89"/>
-      <c r="O10" s="89"/>
-      <c r="P10" s="89"/>
-      <c r="Q10" s="89"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
+      <c r="H10" s="91"/>
+      <c r="I10" s="91"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91"/>
+      <c r="L10" s="91"/>
+      <c r="M10" s="91"/>
+      <c r="N10" s="91"/>
+      <c r="O10" s="91"/>
+      <c r="P10" s="91"/>
+      <c r="Q10" s="91"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>304</v>
       </c>
-      <c r="B11" s="89" t="s">
+      <c r="B11" s="91" t="s">
         <v>170</v>
       </c>
-      <c r="C11" s="89"/>
-      <c r="D11" s="89"/>
-      <c r="E11" s="89"/>
-      <c r="F11" s="89"/>
-      <c r="G11" s="89"/>
-      <c r="H11" s="89"/>
-      <c r="I11" s="89"/>
-      <c r="J11" s="89"/>
-      <c r="K11" s="89"/>
-      <c r="L11" s="89"/>
-      <c r="M11" s="89"/>
-      <c r="N11" s="89"/>
-      <c r="O11" s="89"/>
-      <c r="P11" s="89"/>
-      <c r="Q11" s="89"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="91"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="91"/>
+      <c r="J11" s="91"/>
+      <c r="K11" s="91"/>
+      <c r="L11" s="91"/>
+      <c r="M11" s="91"/>
+      <c r="N11" s="91"/>
+      <c r="O11" s="91"/>
+      <c r="P11" s="91"/>
+      <c r="Q11" s="91"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>305</v>
       </c>
-      <c r="B12" s="89" t="s">
+      <c r="B12" s="91" t="s">
         <v>171</v>
       </c>
-      <c r="C12" s="89"/>
-      <c r="D12" s="89"/>
-      <c r="E12" s="89"/>
-      <c r="F12" s="89"/>
-      <c r="G12" s="89"/>
-      <c r="H12" s="89"/>
-      <c r="I12" s="89"/>
-      <c r="J12" s="89"/>
-      <c r="K12" s="89"/>
-      <c r="L12" s="89"/>
-      <c r="M12" s="89"/>
-      <c r="N12" s="89"/>
-      <c r="O12" s="89"/>
-      <c r="P12" s="89"/>
-      <c r="Q12" s="89"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="91"/>
+      <c r="J12" s="91"/>
+      <c r="K12" s="91"/>
+      <c r="L12" s="91"/>
+      <c r="M12" s="91"/>
+      <c r="N12" s="91"/>
+      <c r="O12" s="91"/>
+      <c r="P12" s="91"/>
+      <c r="Q12" s="91"/>
     </row>
     <row r="13" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="93" t="s">
@@ -3236,24 +3251,24 @@
       <c r="A14" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="91" t="s">
+      <c r="B14" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="89"/>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="89"/>
-      <c r="G14" s="89"/>
-      <c r="H14" s="89"/>
-      <c r="I14" s="89"/>
-      <c r="J14" s="89"/>
-      <c r="K14" s="89"/>
-      <c r="L14" s="89"/>
-      <c r="M14" s="89"/>
-      <c r="N14" s="89"/>
-      <c r="O14" s="89"/>
-      <c r="P14" s="89"/>
-      <c r="Q14" s="89"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="91"/>
+      <c r="G14" s="91"/>
+      <c r="H14" s="91"/>
+      <c r="I14" s="91"/>
+      <c r="J14" s="91"/>
+      <c r="K14" s="91"/>
+      <c r="L14" s="91"/>
+      <c r="M14" s="91"/>
+      <c r="N14" s="91"/>
+      <c r="O14" s="91"/>
+      <c r="P14" s="91"/>
+      <c r="Q14" s="91"/>
     </row>
     <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
@@ -3262,147 +3277,142 @@
       <c r="B15" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="89"/>
-      <c r="D15" s="89"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89"/>
-      <c r="G15" s="89"/>
-      <c r="H15" s="89"/>
-      <c r="I15" s="89"/>
-      <c r="J15" s="89"/>
-      <c r="K15" s="89"/>
-      <c r="L15" s="89"/>
-      <c r="M15" s="89"/>
-      <c r="N15" s="89"/>
-      <c r="O15" s="89"/>
-      <c r="P15" s="89"/>
-      <c r="Q15" s="89"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="91"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="91"/>
+      <c r="J15" s="91"/>
+      <c r="K15" s="91"/>
+      <c r="L15" s="91"/>
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="91"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
     </row>
     <row r="16" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="90" t="s">
+      <c r="A16" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="90"/>
-      <c r="C16" s="90"/>
-      <c r="D16" s="90"/>
-      <c r="E16" s="90"/>
-      <c r="F16" s="90"/>
-      <c r="G16" s="90"/>
-      <c r="H16" s="90"/>
-      <c r="I16" s="90"/>
-      <c r="J16" s="90"/>
-      <c r="K16" s="90"/>
-      <c r="L16" s="90"/>
-      <c r="M16" s="90"/>
-      <c r="N16" s="90"/>
-      <c r="O16" s="90"/>
-      <c r="P16" s="90"/>
-      <c r="Q16" s="90"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="94"/>
+      <c r="D16" s="94"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="94"/>
+      <c r="I16" s="94"/>
+      <c r="J16" s="94"/>
+      <c r="K16" s="94"/>
+      <c r="L16" s="94"/>
+      <c r="M16" s="94"/>
+      <c r="N16" s="94"/>
+      <c r="O16" s="94"/>
+      <c r="P16" s="94"/>
+      <c r="Q16" s="94"/>
     </row>
     <row r="17" spans="1:17" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="94" t="s">
+      <c r="A17" s="95" t="s">
         <v>156</v>
       </c>
-      <c r="B17" s="94"/>
-      <c r="C17" s="94"/>
-      <c r="D17" s="94"/>
-      <c r="E17" s="94"/>
-      <c r="F17" s="94"/>
-      <c r="G17" s="94"/>
-      <c r="H17" s="94"/>
-      <c r="I17" s="94"/>
-      <c r="J17" s="94"/>
-      <c r="K17" s="94"/>
-      <c r="L17" s="94"/>
-      <c r="M17" s="94"/>
-      <c r="N17" s="94"/>
-      <c r="O17" s="94"/>
-      <c r="P17" s="94"/>
-      <c r="Q17" s="94"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="95"/>
+      <c r="G17" s="95"/>
+      <c r="H17" s="95"/>
+      <c r="I17" s="95"/>
+      <c r="J17" s="95"/>
+      <c r="K17" s="95"/>
+      <c r="L17" s="95"/>
+      <c r="M17" s="95"/>
+      <c r="N17" s="95"/>
+      <c r="O17" s="95"/>
+      <c r="P17" s="95"/>
+      <c r="Q17" s="95"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="94"/>
-      <c r="B18" s="94"/>
-      <c r="C18" s="94"/>
-      <c r="D18" s="94"/>
-      <c r="E18" s="94"/>
-      <c r="F18" s="94"/>
-      <c r="G18" s="94"/>
-      <c r="H18" s="94"/>
-      <c r="I18" s="94"/>
-      <c r="J18" s="94"/>
-      <c r="K18" s="94"/>
-      <c r="L18" s="94"/>
-      <c r="M18" s="94"/>
-      <c r="N18" s="94"/>
-      <c r="O18" s="94"/>
-      <c r="P18" s="94"/>
-      <c r="Q18" s="94"/>
+      <c r="A18" s="95"/>
+      <c r="B18" s="95"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="95"/>
+      <c r="F18" s="95"/>
+      <c r="G18" s="95"/>
+      <c r="H18" s="95"/>
+      <c r="I18" s="95"/>
+      <c r="J18" s="95"/>
+      <c r="K18" s="95"/>
+      <c r="L18" s="95"/>
+      <c r="M18" s="95"/>
+      <c r="N18" s="95"/>
+      <c r="O18" s="95"/>
+      <c r="P18" s="95"/>
+      <c r="Q18" s="95"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="94"/>
-      <c r="B19" s="94"/>
-      <c r="C19" s="94"/>
-      <c r="D19" s="94"/>
-      <c r="E19" s="94"/>
-      <c r="F19" s="94"/>
-      <c r="G19" s="94"/>
-      <c r="H19" s="94"/>
-      <c r="I19" s="94"/>
-      <c r="J19" s="94"/>
-      <c r="K19" s="94"/>
-      <c r="L19" s="94"/>
-      <c r="M19" s="94"/>
-      <c r="N19" s="94"/>
-      <c r="O19" s="94"/>
-      <c r="P19" s="94"/>
-      <c r="Q19" s="94"/>
+      <c r="A19" s="95"/>
+      <c r="B19" s="95"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="95"/>
+      <c r="F19" s="95"/>
+      <c r="G19" s="95"/>
+      <c r="H19" s="95"/>
+      <c r="I19" s="95"/>
+      <c r="J19" s="95"/>
+      <c r="K19" s="95"/>
+      <c r="L19" s="95"/>
+      <c r="M19" s="95"/>
+      <c r="N19" s="95"/>
+      <c r="O19" s="95"/>
+      <c r="P19" s="95"/>
+      <c r="Q19" s="95"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="94"/>
-      <c r="B20" s="94"/>
-      <c r="C20" s="94"/>
-      <c r="D20" s="94"/>
-      <c r="E20" s="94"/>
-      <c r="F20" s="94"/>
-      <c r="G20" s="94"/>
-      <c r="H20" s="94"/>
-      <c r="I20" s="94"/>
-      <c r="J20" s="94"/>
-      <c r="K20" s="94"/>
-      <c r="L20" s="94"/>
-      <c r="M20" s="94"/>
-      <c r="N20" s="94"/>
-      <c r="O20" s="94"/>
-      <c r="P20" s="94"/>
-      <c r="Q20" s="94"/>
+      <c r="A20" s="95"/>
+      <c r="B20" s="95"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="95"/>
+      <c r="F20" s="95"/>
+      <c r="G20" s="95"/>
+      <c r="H20" s="95"/>
+      <c r="I20" s="95"/>
+      <c r="J20" s="95"/>
+      <c r="K20" s="95"/>
+      <c r="L20" s="95"/>
+      <c r="M20" s="95"/>
+      <c r="N20" s="95"/>
+      <c r="O20" s="95"/>
+      <c r="P20" s="95"/>
+      <c r="Q20" s="95"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="94"/>
-      <c r="B21" s="94"/>
-      <c r="C21" s="94"/>
-      <c r="D21" s="94"/>
-      <c r="E21" s="94"/>
-      <c r="F21" s="94"/>
-      <c r="G21" s="94"/>
-      <c r="H21" s="94"/>
-      <c r="I21" s="94"/>
-      <c r="J21" s="94"/>
-      <c r="K21" s="94"/>
-      <c r="L21" s="94"/>
-      <c r="M21" s="94"/>
-      <c r="N21" s="94"/>
-      <c r="O21" s="94"/>
-      <c r="P21" s="94"/>
-      <c r="Q21" s="94"/>
+      <c r="A21" s="95"/>
+      <c r="B21" s="95"/>
+      <c r="C21" s="95"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="95"/>
+      <c r="F21" s="95"/>
+      <c r="G21" s="95"/>
+      <c r="H21" s="95"/>
+      <c r="I21" s="95"/>
+      <c r="J21" s="95"/>
+      <c r="K21" s="95"/>
+      <c r="L21" s="95"/>
+      <c r="M21" s="95"/>
+      <c r="N21" s="95"/>
+      <c r="O21" s="95"/>
+      <c r="P21" s="95"/>
+      <c r="Q21" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B14:Q14"/>
-    <mergeCell ref="B15:Q15"/>
-    <mergeCell ref="A13:Q13"/>
-    <mergeCell ref="A16:Q16"/>
-    <mergeCell ref="A17:Q21"/>
     <mergeCell ref="A2:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="B8:M8"/>
@@ -3418,6 +3428,11 @@
     <mergeCell ref="N11:Q11"/>
     <mergeCell ref="N10:Q10"/>
     <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="B14:Q14"/>
+    <mergeCell ref="B15:Q15"/>
+    <mergeCell ref="A13:Q13"/>
+    <mergeCell ref="A16:Q16"/>
+    <mergeCell ref="A17:Q21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B14" r:id="rId1"/>
@@ -3517,8 +3532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3537,142 +3552,142 @@
       <c r="A1" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="96">
+      <c r="B1" s="122">
         <v>301</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="124" t="s">
         <v>172</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="122" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="122"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="123" t="s">
         <v>176</v>
       </c>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="96" t="s">
+      <c r="B7" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="95"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="95"/>
+      <c r="C8" s="123"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="97" t="s">
+      <c r="B9" s="124" t="s">
         <v>157</v>
       </c>
-      <c r="C9" s="96"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="96"/>
+      <c r="C9" s="122"/>
+      <c r="D9" s="122"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="122"/>
     </row>
     <row r="10" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="95" t="s">
+      <c r="B10" s="123" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="95"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="95"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="123"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
     </row>
     <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="103" t="s">
+      <c r="B11" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="103" t="s">
+      <c r="C11" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="105" t="s">
+      <c r="D11" s="107" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="106"/>
-      <c r="F11" s="107"/>
+      <c r="E11" s="108"/>
+      <c r="F11" s="109"/>
     </row>
     <row r="12" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="102"/>
-      <c r="B12" s="104"/>
-      <c r="C12" s="104"/>
+      <c r="A12" s="104"/>
+      <c r="B12" s="106"/>
+      <c r="C12" s="106"/>
       <c r="D12" s="33" t="s">
         <v>17</v>
       </c>
@@ -3717,16 +3732,18 @@
         <v>42855</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="76"/>
       <c r="B15" s="34" t="s">
         <v>163</v>
       </c>
       <c r="C15" s="34"/>
       <c r="D15" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="34"/>
+        <v>9</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>216</v>
+      </c>
       <c r="F15" s="82">
         <v>42855</v>
       </c>
@@ -3861,177 +3878,177 @@
       <c r="A23" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="137">
+      <c r="B23" s="125">
         <v>42855</v>
       </c>
-      <c r="C23" s="98"/>
-      <c r="D23" s="98"/>
-      <c r="E23" s="98"/>
-      <c r="F23" s="99"/>
+      <c r="C23" s="126"/>
+      <c r="D23" s="126"/>
+      <c r="E23" s="126"/>
+      <c r="F23" s="127"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="108" t="s">
+      <c r="A24" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="111"/>
-      <c r="C24" s="112"/>
-      <c r="D24" s="112"/>
-      <c r="E24" s="112"/>
-      <c r="F24" s="113"/>
+      <c r="B24" s="113"/>
+      <c r="C24" s="114"/>
+      <c r="D24" s="114"/>
+      <c r="E24" s="114"/>
+      <c r="F24" s="115"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="109"/>
-      <c r="B25" s="114"/>
-      <c r="C25" s="115"/>
-      <c r="D25" s="115"/>
-      <c r="E25" s="115"/>
-      <c r="F25" s="116"/>
+      <c r="A25" s="111"/>
+      <c r="B25" s="116"/>
+      <c r="C25" s="117"/>
+      <c r="D25" s="117"/>
+      <c r="E25" s="117"/>
+      <c r="F25" s="118"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="109"/>
-      <c r="B26" s="114"/>
-      <c r="C26" s="115"/>
-      <c r="D26" s="115"/>
-      <c r="E26" s="115"/>
-      <c r="F26" s="116"/>
+      <c r="A26" s="111"/>
+      <c r="B26" s="116"/>
+      <c r="C26" s="117"/>
+      <c r="D26" s="117"/>
+      <c r="E26" s="117"/>
+      <c r="F26" s="118"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="109"/>
-      <c r="B27" s="114"/>
-      <c r="C27" s="115"/>
-      <c r="D27" s="115"/>
-      <c r="E27" s="115"/>
-      <c r="F27" s="116"/>
+      <c r="A27" s="111"/>
+      <c r="B27" s="116"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="117"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="118"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="109"/>
-      <c r="B28" s="114"/>
-      <c r="C28" s="115"/>
-      <c r="D28" s="115"/>
-      <c r="E28" s="115"/>
-      <c r="F28" s="116"/>
+      <c r="A28" s="111"/>
+      <c r="B28" s="116"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="117"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="118"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="109"/>
-      <c r="B29" s="114"/>
-      <c r="C29" s="115"/>
-      <c r="D29" s="115"/>
-      <c r="E29" s="115"/>
-      <c r="F29" s="116"/>
+      <c r="A29" s="111"/>
+      <c r="B29" s="116"/>
+      <c r="C29" s="117"/>
+      <c r="D29" s="117"/>
+      <c r="E29" s="117"/>
+      <c r="F29" s="118"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="109"/>
-      <c r="B30" s="114"/>
-      <c r="C30" s="115"/>
-      <c r="D30" s="115"/>
-      <c r="E30" s="115"/>
-      <c r="F30" s="116"/>
+      <c r="A30" s="111"/>
+      <c r="B30" s="116"/>
+      <c r="C30" s="117"/>
+      <c r="D30" s="117"/>
+      <c r="E30" s="117"/>
+      <c r="F30" s="118"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="109"/>
-      <c r="B31" s="114"/>
-      <c r="C31" s="115"/>
-      <c r="D31" s="115"/>
-      <c r="E31" s="115"/>
-      <c r="F31" s="116"/>
+      <c r="A31" s="111"/>
+      <c r="B31" s="116"/>
+      <c r="C31" s="117"/>
+      <c r="D31" s="117"/>
+      <c r="E31" s="117"/>
+      <c r="F31" s="118"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="109"/>
-      <c r="B32" s="114"/>
-      <c r="C32" s="115"/>
-      <c r="D32" s="115"/>
-      <c r="E32" s="115"/>
-      <c r="F32" s="116"/>
+      <c r="A32" s="111"/>
+      <c r="B32" s="116"/>
+      <c r="C32" s="117"/>
+      <c r="D32" s="117"/>
+      <c r="E32" s="117"/>
+      <c r="F32" s="118"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="109"/>
-      <c r="B33" s="114"/>
-      <c r="C33" s="115"/>
-      <c r="D33" s="115"/>
-      <c r="E33" s="115"/>
-      <c r="F33" s="116"/>
+      <c r="A33" s="111"/>
+      <c r="B33" s="116"/>
+      <c r="C33" s="117"/>
+      <c r="D33" s="117"/>
+      <c r="E33" s="117"/>
+      <c r="F33" s="118"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="109"/>
-      <c r="B34" s="114"/>
-      <c r="C34" s="115"/>
-      <c r="D34" s="115"/>
-      <c r="E34" s="115"/>
-      <c r="F34" s="116"/>
+      <c r="A34" s="111"/>
+      <c r="B34" s="116"/>
+      <c r="C34" s="117"/>
+      <c r="D34" s="117"/>
+      <c r="E34" s="117"/>
+      <c r="F34" s="118"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="109"/>
-      <c r="B35" s="114"/>
-      <c r="C35" s="115"/>
-      <c r="D35" s="115"/>
-      <c r="E35" s="115"/>
-      <c r="F35" s="116"/>
+      <c r="A35" s="111"/>
+      <c r="B35" s="116"/>
+      <c r="C35" s="117"/>
+      <c r="D35" s="117"/>
+      <c r="E35" s="117"/>
+      <c r="F35" s="118"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="109"/>
-      <c r="B36" s="114"/>
-      <c r="C36" s="115"/>
-      <c r="D36" s="115"/>
-      <c r="E36" s="115"/>
-      <c r="F36" s="116"/>
+      <c r="A36" s="111"/>
+      <c r="B36" s="116"/>
+      <c r="C36" s="117"/>
+      <c r="D36" s="117"/>
+      <c r="E36" s="117"/>
+      <c r="F36" s="118"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="109"/>
-      <c r="B37" s="114"/>
-      <c r="C37" s="115"/>
-      <c r="D37" s="115"/>
-      <c r="E37" s="115"/>
-      <c r="F37" s="116"/>
+      <c r="A37" s="111"/>
+      <c r="B37" s="116"/>
+      <c r="C37" s="117"/>
+      <c r="D37" s="117"/>
+      <c r="E37" s="117"/>
+      <c r="F37" s="118"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="109"/>
-      <c r="B38" s="114"/>
-      <c r="C38" s="115"/>
-      <c r="D38" s="115"/>
-      <c r="E38" s="115"/>
-      <c r="F38" s="116"/>
+      <c r="A38" s="111"/>
+      <c r="B38" s="116"/>
+      <c r="C38" s="117"/>
+      <c r="D38" s="117"/>
+      <c r="E38" s="117"/>
+      <c r="F38" s="118"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="109"/>
-      <c r="B39" s="114"/>
-      <c r="C39" s="115"/>
-      <c r="D39" s="115"/>
-      <c r="E39" s="115"/>
-      <c r="F39" s="116"/>
+      <c r="A39" s="111"/>
+      <c r="B39" s="116"/>
+      <c r="C39" s="117"/>
+      <c r="D39" s="117"/>
+      <c r="E39" s="117"/>
+      <c r="F39" s="118"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="109"/>
-      <c r="B40" s="114"/>
-      <c r="C40" s="115"/>
-      <c r="D40" s="115"/>
-      <c r="E40" s="115"/>
-      <c r="F40" s="116"/>
+      <c r="A40" s="111"/>
+      <c r="B40" s="116"/>
+      <c r="C40" s="117"/>
+      <c r="D40" s="117"/>
+      <c r="E40" s="117"/>
+      <c r="F40" s="118"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="109"/>
-      <c r="B41" s="114"/>
-      <c r="C41" s="115"/>
-      <c r="D41" s="115"/>
-      <c r="E41" s="115"/>
-      <c r="F41" s="116"/>
+      <c r="A41" s="111"/>
+      <c r="B41" s="116"/>
+      <c r="C41" s="117"/>
+      <c r="D41" s="117"/>
+      <c r="E41" s="117"/>
+      <c r="F41" s="118"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="110"/>
-      <c r="B42" s="117"/>
-      <c r="C42" s="118"/>
-      <c r="D42" s="118"/>
-      <c r="E42" s="118"/>
-      <c r="F42" s="119"/>
+      <c r="A42" s="112"/>
+      <c r="B42" s="119"/>
+      <c r="C42" s="120"/>
+      <c r="D42" s="120"/>
+      <c r="E42" s="120"/>
+      <c r="F42" s="121"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="100" t="s">
+      <c r="A43" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="100"/>
-      <c r="C43" s="100"/>
-      <c r="D43" s="100"/>
-      <c r="E43" s="100"/>
-      <c r="F43" s="100"/>
+      <c r="B43" s="102"/>
+      <c r="C43" s="102"/>
+      <c r="D43" s="102"/>
+      <c r="E43" s="102"/>
+      <c r="F43" s="102"/>
     </row>
     <row r="44" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="23" t="s">
@@ -4143,6 +4160,17 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B23:F23"/>
     <mergeCell ref="A43:F43"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
@@ -4150,17 +4178,6 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="A24:A42"/>
     <mergeCell ref="B24:F42"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
   </mergeCells>
   <conditionalFormatting sqref="D13:D22">
     <cfRule type="cellIs" dxfId="69" priority="5" stopIfTrue="1" operator="equal">
@@ -4210,8 +4227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4231,169 +4248,169 @@
       <c r="A1" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="96">
+      <c r="B1" s="122">
         <v>302</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="124" t="s">
         <v>168</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="122" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="122"/>
+      <c r="G4" s="122"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="123" t="s">
         <v>176</v>
       </c>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="123"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="123"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="96" t="s">
+      <c r="B7" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="122"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="95"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="95"/>
-      <c r="G8" s="95"/>
+      <c r="C8" s="123"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="123"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="97" t="s">
+      <c r="B9" s="124" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="96"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="96"/>
-      <c r="G9" s="96"/>
+      <c r="C9" s="122"/>
+      <c r="D9" s="122"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="122"/>
+      <c r="G9" s="122"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="95" t="s">
+      <c r="B10" s="123" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="95"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="95"/>
-      <c r="G10" s="95"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="123"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="123"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="B11" s="120" t="s">
+      <c r="B11" s="136" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="120"/>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
-      <c r="G11" s="120"/>
+      <c r="C11" s="136"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="136"/>
+      <c r="F11" s="136"/>
+      <c r="G11" s="136"/>
     </row>
     <row r="12" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="101" t="s">
+      <c r="A12" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="103" t="s">
+      <c r="B12" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="124" t="s">
+      <c r="C12" s="131" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="103" t="s">
+      <c r="D12" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="105" t="s">
+      <c r="E12" s="107" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="106"/>
-      <c r="G12" s="107"/>
+      <c r="F12" s="108"/>
+      <c r="G12" s="109"/>
     </row>
     <row r="13" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="122"/>
-      <c r="B13" s="123"/>
-      <c r="C13" s="125"/>
-      <c r="D13" s="104"/>
+      <c r="A13" s="129"/>
+      <c r="B13" s="130"/>
+      <c r="C13" s="132"/>
+      <c r="D13" s="106"/>
       <c r="E13" s="32" t="s">
         <v>17</v>
       </c>
@@ -4421,7 +4438,7 @@
       <c r="F14" s="39" t="s">
         <v>182</v>
       </c>
-      <c r="G14" s="136">
+      <c r="G14" s="83">
         <v>42856</v>
       </c>
     </row>
@@ -4440,7 +4457,7 @@
       <c r="F15" s="39" t="s">
         <v>182</v>
       </c>
-      <c r="G15" s="136">
+      <c r="G15" s="83">
         <v>42856</v>
       </c>
     </row>
@@ -4461,7 +4478,7 @@
       <c r="F16" s="39" t="s">
         <v>182</v>
       </c>
-      <c r="G16" s="136">
+      <c r="G16" s="83">
         <v>42856</v>
       </c>
     </row>
@@ -4480,7 +4497,7 @@
         <v>7</v>
       </c>
       <c r="F17" s="42"/>
-      <c r="G17" s="136">
+      <c r="G17" s="83">
         <v>42856</v>
       </c>
     </row>
@@ -4496,10 +4513,12 @@
       </c>
       <c r="D18" s="34"/>
       <c r="E18" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="42"/>
-      <c r="G18" s="136">
+        <v>9</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>218</v>
+      </c>
+      <c r="G18" s="83">
         <v>42856</v>
       </c>
     </row>
@@ -4518,7 +4537,7 @@
         <v>7</v>
       </c>
       <c r="F19" s="42"/>
-      <c r="G19" s="136">
+      <c r="G19" s="83">
         <v>42856</v>
       </c>
     </row>
@@ -4535,7 +4554,7 @@
         <v>7</v>
       </c>
       <c r="F20" s="42"/>
-      <c r="G20" s="136">
+      <c r="G20" s="83">
         <v>42856</v>
       </c>
     </row>
@@ -4554,7 +4573,7 @@
         <v>7</v>
       </c>
       <c r="F21" s="42"/>
-      <c r="G21" s="136">
+      <c r="G21" s="83">
         <v>42856</v>
       </c>
     </row>
@@ -4570,10 +4589,12 @@
       </c>
       <c r="D22" s="34"/>
       <c r="E22" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="42"/>
-      <c r="G22" s="136">
+        <v>9</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="G22" s="83">
         <v>42856</v>
       </c>
     </row>
@@ -4592,7 +4613,7 @@
         <v>7</v>
       </c>
       <c r="F23" s="42"/>
-      <c r="G23" s="136">
+      <c r="G23" s="83">
         <v>42856</v>
       </c>
     </row>
@@ -4609,7 +4630,7 @@
         <v>7</v>
       </c>
       <c r="F24" s="42"/>
-      <c r="G24" s="136">
+      <c r="G24" s="83">
         <v>42856</v>
       </c>
     </row>
@@ -4628,7 +4649,7 @@
         <v>7</v>
       </c>
       <c r="F25" s="42"/>
-      <c r="G25" s="136">
+      <c r="G25" s="83">
         <v>42856</v>
       </c>
     </row>
@@ -4645,7 +4666,7 @@
         <v>7</v>
       </c>
       <c r="F26" s="42"/>
-      <c r="G26" s="136">
+      <c r="G26" s="83">
         <v>42856</v>
       </c>
     </row>
@@ -4664,7 +4685,7 @@
         <v>7</v>
       </c>
       <c r="F27" s="42"/>
-      <c r="G27" s="136">
+      <c r="G27" s="83">
         <v>42856</v>
       </c>
     </row>
@@ -4680,10 +4701,12 @@
       </c>
       <c r="D28" s="50"/>
       <c r="E28" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="49"/>
-      <c r="G28" s="136">
+        <v>9</v>
+      </c>
+      <c r="F28" s="50" t="s">
+        <v>219</v>
+      </c>
+      <c r="G28" s="83">
         <v>42856</v>
       </c>
     </row>
@@ -4691,25 +4714,25 @@
       <c r="A29" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="98" t="s">
+      <c r="B29" s="126" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="98"/>
-      <c r="D29" s="98"/>
-      <c r="E29" s="98"/>
-      <c r="F29" s="98"/>
-      <c r="G29" s="99"/>
+      <c r="C29" s="126"/>
+      <c r="D29" s="126"/>
+      <c r="E29" s="126"/>
+      <c r="F29" s="126"/>
+      <c r="G29" s="127"/>
     </row>
     <row r="30" spans="1:7" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="144"/>
-      <c r="C30" s="127"/>
-      <c r="D30" s="127"/>
-      <c r="E30" s="127"/>
-      <c r="F30" s="127"/>
-      <c r="G30" s="128"/>
+      <c r="B30" s="133"/>
+      <c r="C30" s="134"/>
+      <c r="D30" s="134"/>
+      <c r="E30" s="134"/>
+      <c r="F30" s="134"/>
+      <c r="G30" s="135"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="21"/>
@@ -4721,15 +4744,15 @@
       <c r="G31" s="22"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="121" t="s">
+      <c r="A32" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="121"/>
-      <c r="C32" s="121"/>
-      <c r="D32" s="121"/>
-      <c r="E32" s="121"/>
-      <c r="F32" s="121"/>
-      <c r="G32" s="121"/>
+      <c r="B32" s="128"/>
+      <c r="C32" s="128"/>
+      <c r="D32" s="128"/>
+      <c r="E32" s="128"/>
+      <c r="F32" s="128"/>
+      <c r="G32" s="128"/>
     </row>
     <row r="33" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="23" t="s">
@@ -4835,6 +4858,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B11:G11"/>
     <mergeCell ref="A32:G32"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
@@ -4842,18 +4877,6 @@
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
   </mergeCells>
   <conditionalFormatting sqref="E14:E28">
     <cfRule type="cellIs" dxfId="60" priority="9" stopIfTrue="1" operator="equal">
@@ -4903,8 +4926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4922,154 +4945,154 @@
       <c r="A1" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="96">
+      <c r="B1" s="122">
         <v>303</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="124" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="122" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="122"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="123" t="s">
         <v>176</v>
       </c>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="96" t="s">
+      <c r="B7" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="95"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="95"/>
+      <c r="C8" s="123"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="97" t="s">
+      <c r="B9" s="124" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="96"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="96"/>
+      <c r="C9" s="122"/>
+      <c r="D9" s="122"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="122"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="95" t="s">
+      <c r="B10" s="123" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="95"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="95"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="123"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="B11" s="120" t="s">
+      <c r="B11" s="136" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="120"/>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
+      <c r="C11" s="136"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="136"/>
+      <c r="F11" s="136"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="101" t="s">
+      <c r="A12" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="103" t="s">
+      <c r="B12" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="124" t="s">
+      <c r="C12" s="131" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="105" t="s">
+      <c r="D12" s="107" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="106"/>
-      <c r="F12" s="107"/>
+      <c r="E12" s="108"/>
+      <c r="F12" s="109"/>
     </row>
     <row r="13" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="102"/>
-      <c r="B13" s="104"/>
-      <c r="C13" s="129"/>
+      <c r="A13" s="104"/>
+      <c r="B13" s="106"/>
+      <c r="C13" s="138"/>
       <c r="D13" s="33" t="s">
         <v>17</v>
       </c>
@@ -5094,7 +5117,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="39"/>
-      <c r="F14" s="136">
+      <c r="F14" s="83">
         <v>42856</v>
       </c>
     </row>
@@ -5160,7 +5183,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="29"/>
-      <c r="F18" s="138">
+      <c r="F18" s="84">
         <v>42856</v>
       </c>
     </row>
@@ -5168,25 +5191,25 @@
       <c r="A19" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="127" t="s">
+      <c r="B19" s="134" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="127"/>
-      <c r="D19" s="127"/>
-      <c r="E19" s="127"/>
-      <c r="F19" s="128"/>
+      <c r="C19" s="134"/>
+      <c r="D19" s="134"/>
+      <c r="E19" s="134"/>
+      <c r="F19" s="135"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="126" t="s">
+      <c r="B20" s="137" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="127"/>
-      <c r="D20" s="127"/>
-      <c r="E20" s="127"/>
-      <c r="F20" s="128"/>
+      <c r="C20" s="134"/>
+      <c r="D20" s="134"/>
+      <c r="E20" s="134"/>
+      <c r="F20" s="135"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21"/>
@@ -5197,14 +5220,14 @@
       <c r="F21" s="22"/>
     </row>
     <row r="22" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="121" t="s">
+      <c r="A22" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="121"/>
-      <c r="C22" s="121"/>
-      <c r="D22" s="121"/>
-      <c r="E22" s="121"/>
-      <c r="F22" s="121"/>
+      <c r="B22" s="128"/>
+      <c r="C22" s="128"/>
+      <c r="D22" s="128"/>
+      <c r="E22" s="128"/>
+      <c r="F22" s="128"/>
     </row>
     <row r="23" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="23" t="s">
@@ -5268,24 +5291,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B11:F11"/>
     <mergeCell ref="A22:F22"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:F12"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
   </mergeCells>
   <conditionalFormatting sqref="D14:D18">
     <cfRule type="cellIs" dxfId="51" priority="5" stopIfTrue="1" operator="equal">
@@ -5334,7 +5357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -5354,154 +5377,154 @@
       <c r="A1" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="96">
+      <c r="B1" s="122">
         <v>304</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="124" t="s">
         <v>170</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="122" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="122"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="123" t="s">
         <v>176</v>
       </c>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="96" t="s">
+      <c r="B7" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="123" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="95"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="95"/>
+      <c r="C8" s="123"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="97" t="s">
+      <c r="B9" s="124" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="96"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="96"/>
+      <c r="C9" s="122"/>
+      <c r="D9" s="122"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="122"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="95" t="s">
+      <c r="B10" s="123" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="95"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="95"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="123"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="B11" s="120" t="s">
+      <c r="B11" s="136" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="120"/>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
+      <c r="C11" s="136"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="136"/>
+      <c r="F11" s="136"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="101" t="s">
+      <c r="A12" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="103" t="s">
+      <c r="B12" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="124" t="s">
+      <c r="C12" s="131" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="105" t="s">
+      <c r="D12" s="107" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="106"/>
-      <c r="F12" s="107"/>
+      <c r="E12" s="108"/>
+      <c r="F12" s="109"/>
     </row>
     <row r="13" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="102"/>
-      <c r="B13" s="104"/>
-      <c r="C13" s="129"/>
+      <c r="A13" s="104"/>
+      <c r="B13" s="106"/>
+      <c r="C13" s="138"/>
       <c r="D13" s="33" t="s">
         <v>17</v>
       </c>
@@ -5624,25 +5647,25 @@
       <c r="A21" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="127" t="s">
+      <c r="B21" s="134" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="127"/>
-      <c r="D21" s="127"/>
-      <c r="E21" s="127"/>
-      <c r="F21" s="128"/>
+      <c r="C21" s="134"/>
+      <c r="D21" s="134"/>
+      <c r="E21" s="134"/>
+      <c r="F21" s="135"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="126" t="s">
+      <c r="B22" s="137" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="127"/>
-      <c r="D22" s="127"/>
-      <c r="E22" s="127"/>
-      <c r="F22" s="128"/>
+      <c r="C22" s="134"/>
+      <c r="D22" s="134"/>
+      <c r="E22" s="134"/>
+      <c r="F22" s="135"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21"/>
@@ -5653,14 +5676,14 @@
       <c r="F23" s="22"/>
     </row>
     <row r="24" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="121" t="s">
+      <c r="A24" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="121"/>
-      <c r="C24" s="121"/>
-      <c r="D24" s="121"/>
-      <c r="E24" s="121"/>
-      <c r="F24" s="121"/>
+      <c r="B24" s="128"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="128"/>
+      <c r="E24" s="128"/>
+      <c r="F24" s="128"/>
     </row>
     <row r="25" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="23" t="s">
@@ -5724,24 +5747,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B11:F11"/>
     <mergeCell ref="A24:F24"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:F12"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
   </mergeCells>
   <conditionalFormatting sqref="D14:D20">
     <cfRule type="cellIs" dxfId="42" priority="5" stopIfTrue="1" operator="equal">
@@ -5790,7 +5813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -5814,164 +5837,164 @@
       <c r="A1" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="122"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="122" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="122"/>
+      <c r="L2" s="122"/>
+      <c r="M2" s="122"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="122"/>
+      <c r="K3" s="122"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="122"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="95"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="95"/>
-      <c r="H4" s="95"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="95"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="95"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
+      <c r="G4" s="123"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="123"/>
+      <c r="M4" s="123"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="97" t="s">
+      <c r="B5" s="124" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
-      <c r="K5" s="97"/>
-      <c r="L5" s="97"/>
-      <c r="M5" s="97"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="124"/>
+      <c r="F5" s="124"/>
+      <c r="G5" s="124"/>
+      <c r="H5" s="124"/>
+      <c r="I5" s="124"/>
+      <c r="J5" s="124"/>
+      <c r="K5" s="124"/>
+      <c r="L5" s="124"/>
+      <c r="M5" s="124"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="73" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="132" t="s">
+      <c r="B6" s="141" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="132"/>
-      <c r="D6" s="132"/>
-      <c r="E6" s="132"/>
-      <c r="F6" s="132"/>
-      <c r="G6" s="132"/>
-      <c r="H6" s="132"/>
-      <c r="I6" s="132"/>
-      <c r="J6" s="132"/>
-      <c r="K6" s="132"/>
-      <c r="L6" s="132"/>
-      <c r="M6" s="132"/>
+      <c r="C6" s="141"/>
+      <c r="D6" s="141"/>
+      <c r="E6" s="141"/>
+      <c r="F6" s="141"/>
+      <c r="G6" s="141"/>
+      <c r="H6" s="141"/>
+      <c r="I6" s="141"/>
+      <c r="J6" s="141"/>
+      <c r="K6" s="141"/>
+      <c r="L6" s="141"/>
+      <c r="M6" s="141"/>
     </row>
     <row r="7" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="101" t="s">
+      <c r="A7" s="103" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="130" t="s">
+      <c r="B7" s="139" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="130" t="s">
+      <c r="C7" s="139" t="s">
         <v>98</v>
       </c>
-      <c r="D7" s="130" t="s">
+      <c r="D7" s="139" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="130" t="s">
+      <c r="E7" s="139" t="s">
         <v>100</v>
       </c>
-      <c r="F7" s="130" t="s">
+      <c r="F7" s="139" t="s">
         <v>101</v>
       </c>
-      <c r="G7" s="103" t="s">
+      <c r="G7" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="103" t="s">
+      <c r="H7" s="105" t="s">
         <v>106</v>
       </c>
-      <c r="I7" s="103" t="s">
+      <c r="I7" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="124" t="s">
+      <c r="J7" s="131" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="105" t="s">
+      <c r="K7" s="107" t="s">
         <v>55</v>
       </c>
-      <c r="L7" s="106"/>
-      <c r="M7" s="107"/>
+      <c r="L7" s="108"/>
+      <c r="M7" s="109"/>
     </row>
     <row r="8" spans="1:13" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="102"/>
-      <c r="B8" s="131"/>
-      <c r="C8" s="131"/>
-      <c r="D8" s="131"/>
-      <c r="E8" s="131"/>
-      <c r="F8" s="131"/>
-      <c r="G8" s="104"/>
-      <c r="H8" s="104"/>
-      <c r="I8" s="104"/>
-      <c r="J8" s="129"/>
+      <c r="A8" s="104"/>
+      <c r="B8" s="140"/>
+      <c r="C8" s="140"/>
+      <c r="D8" s="140"/>
+      <c r="E8" s="140"/>
+      <c r="F8" s="140"/>
+      <c r="G8" s="106"/>
+      <c r="H8" s="106"/>
+      <c r="I8" s="106"/>
+      <c r="J8" s="138"/>
       <c r="K8" s="33" t="s">
         <v>97</v>
       </c>
@@ -6013,7 +6036,7 @@
         <v>7</v>
       </c>
       <c r="L9" s="37"/>
-      <c r="M9" s="139">
+      <c r="M9" s="85">
         <v>42856</v>
       </c>
     </row>
@@ -6054,7 +6077,7 @@
       <c r="L10" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="M10" s="140">
+      <c r="M10" s="86">
         <v>42856</v>
       </c>
     </row>
@@ -6089,7 +6112,7 @@
         <v>7</v>
       </c>
       <c r="L11" s="34"/>
-      <c r="M11" s="140">
+      <c r="M11" s="86">
         <v>42856</v>
       </c>
     </row>
@@ -6126,7 +6149,7 @@
         <v>7</v>
       </c>
       <c r="L12" s="34"/>
-      <c r="M12" s="140">
+      <c r="M12" s="86">
         <v>42856</v>
       </c>
     </row>
@@ -6163,7 +6186,7 @@
         <v>7</v>
       </c>
       <c r="L13" s="34"/>
-      <c r="M13" s="140">
+      <c r="M13" s="86">
         <v>42856</v>
       </c>
     </row>
@@ -6202,7 +6225,7 @@
       <c r="L14" s="80" t="s">
         <v>211</v>
       </c>
-      <c r="M14" s="141">
+      <c r="M14" s="87">
         <v>42856</v>
       </c>
     </row>
@@ -6237,7 +6260,7 @@
         <v>7</v>
       </c>
       <c r="L15" s="37"/>
-      <c r="M15" s="139">
+      <c r="M15" s="85">
         <v>42856</v>
       </c>
     </row>
@@ -6272,7 +6295,7 @@
         <v>7</v>
       </c>
       <c r="L16" s="34"/>
-      <c r="M16" s="140">
+      <c r="M16" s="86">
         <v>42856</v>
       </c>
     </row>
@@ -6307,7 +6330,7 @@
         <v>7</v>
       </c>
       <c r="L17" s="50"/>
-      <c r="M17" s="142">
+      <c r="M17" s="88">
         <v>42856</v>
       </c>
     </row>
@@ -6342,17 +6365,12 @@
         <v>7</v>
       </c>
       <c r="L18" s="68"/>
-      <c r="M18" s="143">
+      <c r="M18" s="89">
         <v>42856</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="B1:M1"/>
-    <mergeCell ref="B2:M2"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="J7:J8"/>
@@ -6360,11 +6378,16 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:M3"/>
     <mergeCell ref="B4:M4"/>
-    <mergeCell ref="H7:H8"/>
     <mergeCell ref="B6:M6"/>
-    <mergeCell ref="I7:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="K9:K18">
     <cfRule type="cellIs" dxfId="33" priority="5" stopIfTrue="1" operator="equal">
@@ -6423,111 +6446,111 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="133" t="s">
+      <c r="B1" s="142" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="133"/>
-      <c r="D1" s="133"/>
-      <c r="E1" s="133"/>
-      <c r="F1" s="133"/>
-      <c r="G1" s="133"/>
-      <c r="H1" s="133"/>
-      <c r="I1" s="133"/>
-      <c r="J1" s="133"/>
-      <c r="K1" s="133"/>
-      <c r="L1" s="133"/>
-      <c r="M1" s="133"/>
-      <c r="N1" s="133"/>
-      <c r="O1" s="133"/>
-      <c r="P1" s="133"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142"/>
+      <c r="K1" s="142"/>
+      <c r="L1" s="142"/>
+      <c r="M1" s="142"/>
+      <c r="N1" s="142"/>
+      <c r="O1" s="142"/>
+      <c r="P1" s="142"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="134" t="s">
+      <c r="B2" s="143" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="134"/>
-      <c r="L2" s="134"/>
-      <c r="M2" s="134"/>
-      <c r="N2" s="134"/>
-      <c r="O2" s="134"/>
-      <c r="P2" s="134"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
+      <c r="H2" s="143"/>
+      <c r="I2" s="143"/>
+      <c r="J2" s="143"/>
+      <c r="K2" s="143"/>
+      <c r="L2" s="143"/>
+      <c r="M2" s="143"/>
+      <c r="N2" s="143"/>
+      <c r="O2" s="143"/>
+      <c r="P2" s="143"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="135" t="s">
+      <c r="B3" s="144" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="135"/>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="135"/>
-      <c r="K3" s="135"/>
-      <c r="L3" s="135"/>
-      <c r="M3" s="135"/>
-      <c r="N3" s="135"/>
-      <c r="O3" s="135"/>
-      <c r="P3" s="135"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="144"/>
+      <c r="K3" s="144"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="144"/>
+      <c r="O3" s="144"/>
+      <c r="P3" s="144"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="134" t="s">
+      <c r="B4" s="143" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="134"/>
-      <c r="D4" s="134"/>
-      <c r="E4" s="134"/>
-      <c r="F4" s="134"/>
-      <c r="G4" s="134"/>
-      <c r="H4" s="134"/>
-      <c r="I4" s="134"/>
-      <c r="J4" s="134"/>
-      <c r="K4" s="134"/>
-      <c r="L4" s="134"/>
-      <c r="M4" s="134"/>
-      <c r="N4" s="134"/>
-      <c r="O4" s="134"/>
-      <c r="P4" s="134"/>
+      <c r="C4" s="143"/>
+      <c r="D4" s="143"/>
+      <c r="E4" s="143"/>
+      <c r="F4" s="143"/>
+      <c r="G4" s="143"/>
+      <c r="H4" s="143"/>
+      <c r="I4" s="143"/>
+      <c r="J4" s="143"/>
+      <c r="K4" s="143"/>
+      <c r="L4" s="143"/>
+      <c r="M4" s="143"/>
+      <c r="N4" s="143"/>
+      <c r="O4" s="143"/>
+      <c r="P4" s="143"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="133" t="s">
+      <c r="B5" s="142" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="133"/>
-      <c r="D5" s="133"/>
-      <c r="E5" s="133"/>
-      <c r="F5" s="133"/>
-      <c r="G5" s="133"/>
-      <c r="H5" s="133"/>
-      <c r="I5" s="133"/>
-      <c r="J5" s="133"/>
-      <c r="K5" s="133"/>
-      <c r="L5" s="133"/>
-      <c r="M5" s="133"/>
-      <c r="N5" s="133"/>
-      <c r="O5" s="133"/>
-      <c r="P5" s="133"/>
+      <c r="C5" s="142"/>
+      <c r="D5" s="142"/>
+      <c r="E5" s="142"/>
+      <c r="F5" s="142"/>
+      <c r="G5" s="142"/>
+      <c r="H5" s="142"/>
+      <c r="I5" s="142"/>
+      <c r="J5" s="142"/>
+      <c r="K5" s="142"/>
+      <c r="L5" s="142"/>
+      <c r="M5" s="142"/>
+      <c r="N5" s="142"/>
+      <c r="O5" s="142"/>
+      <c r="P5" s="142"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>